<commit_message>
add urls, improve filtering by pack, add category select
</commit_message>
<xml_diff>
--- a/JackBox.xlsx
+++ b/JackBox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JessicaMulein\source\repos\jackbase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2118775-226B-4214-95CC-EB78AA6BC783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD78104-2D73-4B5E-B268-41189F70FFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5010" yWindow="90" windowWidth="19950" windowHeight="11650" xr2:uid="{4A7DAA00-A669-425F-B46F-0302A9CBEEA0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="169">
   <si>
     <t>Game</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Trivia Murder Party 2</t>
   </si>
   <si>
-    <t>dictionarium</t>
-  </si>
-  <si>
     <t>The Devils and the Details</t>
   </si>
   <si>
@@ -212,18 +209,9 @@
     <t>Fibbage 4</t>
   </si>
   <si>
-    <t>Fixy Text</t>
-  </si>
-  <si>
     <t>Tee K.O. 2</t>
   </si>
   <si>
-    <t>DodoReMi</t>
-  </si>
-  <si>
-    <t>Time Jinx</t>
-  </si>
-  <si>
     <t>Hypnotorious</t>
   </si>
   <si>
@@ -390,13 +378,178 @@
   </si>
   <si>
     <t>max Players</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/fibbage-xl</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/lie-swatter</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/word-spud</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/quiplash-xl</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/bomb-corp</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/civic-doodle</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/patently-stupid</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/you-dont-know-jack-2015</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/drawful</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/earwax</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/bidiots</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/guesspionage</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/bracketeering</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/fibbage-2</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/tee-k-o</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/quiplash-2-1</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/trivia-murder-party</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/fakin-it</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/fibbage-3</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/survive-the-internet</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/monster-seeking-monster</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/mad-verse-city</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/you-dont-know-jack-full-stream</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/split-the-room</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/zeeple-dome</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/role-models</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/push-the-button</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/joke-boat</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/trivia-murder-party-2</t>
+  </si>
+  <si>
+    <t>Dictionarium</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/dictionarium</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/devils-and-the-details</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/champd-up</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/talking-points</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/quiplash-3</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/blather-round</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/job-job</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/weapons-drawn</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/drawful-animate</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/poll-mine</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/the-wheel-of-enormous-proportions</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/junktopia</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/quixort</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/roomerang</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/nonsensory</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/fibbage-4</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/fixytext</t>
+  </si>
+  <si>
+    <t>FixyText</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/tee-k-o-2</t>
+  </si>
+  <si>
+    <t>Dodo Re Mi</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/dodo-re-mi</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/timejinx</t>
+  </si>
+  <si>
+    <t>Timejinx</t>
+  </si>
+  <si>
+    <t>https://www.jackboxgames.com/games/hypnotorious</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +561,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -436,10 +597,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -461,8 +623,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -775,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CE10CE-68E0-403A-9300-8085A303CF36}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -788,10 +953,10 @@
     <col min="3" max="3" width="11" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.90625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="8"/>
-    <col min="6" max="6" width="12.54296875" customWidth="1"/>
+    <col min="6" max="7" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -799,10 +964,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -811,10 +976,13 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -833,11 +1001,14 @@
       <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -856,11 +1027,14 @@
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -879,11 +1053,14 @@
       <c r="F4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -900,11 +1077,14 @@
       <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -921,11 +1101,14 @@
       <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -944,11 +1127,14 @@
       <c r="F7" t="s">
         <v>15</v>
       </c>
-      <c r="G7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -967,11 +1153,14 @@
       <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G8" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -990,13 +1179,16 @@
       <c r="F9" t="s">
         <v>12</v>
       </c>
-      <c r="G9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G9" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
@@ -1013,11 +1205,14 @@
       <c r="F10" t="s">
         <v>14</v>
       </c>
-      <c r="G10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G10" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1036,11 +1231,14 @@
       <c r="F11" t="s">
         <v>19</v>
       </c>
-      <c r="G11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -1059,11 +1257,14 @@
       <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G12" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
@@ -1082,11 +1283,14 @@
       <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>22</v>
       </c>
@@ -1105,11 +1309,14 @@
       <c r="F14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
@@ -1128,11 +1335,14 @@
       <c r="F15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>24</v>
       </c>
@@ -1151,11 +1361,14 @@
       <c r="F16" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G16" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1174,11 +1387,14 @@
       <c r="F17" t="s">
         <v>11</v>
       </c>
-      <c r="G17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G17" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="H17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1197,11 +1413,14 @@
       <c r="F18" t="s">
         <v>14</v>
       </c>
-      <c r="G18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G18" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1220,11 +1439,14 @@
       <c r="F19" t="s">
         <v>29</v>
       </c>
-      <c r="G19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G19" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1243,11 +1465,14 @@
       <c r="F20" t="s">
         <v>12</v>
       </c>
-      <c r="G20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G20" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="H20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1266,11 +1491,14 @@
       <c r="F21" t="s">
         <v>25</v>
       </c>
-      <c r="G21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>32</v>
       </c>
@@ -1289,11 +1517,14 @@
       <c r="F22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
@@ -1312,11 +1543,14 @@
       <c r="F23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>34</v>
       </c>
@@ -1335,11 +1569,14 @@
       <c r="F24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
@@ -1358,11 +1595,14 @@
       <c r="F25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>36</v>
       </c>
@@ -1381,11 +1621,14 @@
       <c r="F26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G26" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1404,11 +1647,14 @@
       <c r="F27" t="s">
         <v>25</v>
       </c>
-      <c r="G27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G27" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1427,11 +1673,14 @@
       <c r="F28" t="s">
         <v>11</v>
       </c>
-      <c r="G28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G28" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1450,11 +1699,14 @@
       <c r="F29" t="s">
         <v>41</v>
       </c>
-      <c r="G29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G29" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="H29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1473,13 +1725,16 @@
       <c r="F30" t="s">
         <v>10</v>
       </c>
-      <c r="G30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G30" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="H30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>144</v>
       </c>
       <c r="B31" s="1">
         <v>6</v>
@@ -1496,13 +1751,16 @@
       <c r="F31" t="s">
         <v>14</v>
       </c>
-      <c r="G31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G31" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" s="5">
         <v>7</v>
@@ -1519,13 +1777,16 @@
       <c r="F32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G32" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" s="5">
         <v>7</v>
@@ -1542,13 +1803,16 @@
       <c r="F33" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G33" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G33" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="5">
         <v>7</v>
@@ -1565,13 +1829,16 @@
       <c r="F34" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G34" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G34" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="5">
         <v>7</v>
@@ -1588,13 +1855,16 @@
       <c r="F35" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G35" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" s="5">
         <v>7</v>
@@ -1611,13 +1881,16 @@
       <c r="F36" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G36" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B37" s="1">
         <v>8</v>
@@ -1634,13 +1907,16 @@
       <c r="F37" t="s">
         <v>14</v>
       </c>
-      <c r="G37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G37" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="H37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" s="1">
         <v>8</v>
@@ -1657,13 +1933,16 @@
       <c r="F38" t="s">
         <v>12</v>
       </c>
-      <c r="G38" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G38" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B39" s="1">
         <v>8</v>
@@ -1680,13 +1959,16 @@
       <c r="F39" t="s">
         <v>12</v>
       </c>
-      <c r="G39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G39" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="H39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B40" s="1">
         <v>8</v>
@@ -1703,13 +1985,16 @@
       <c r="F40" t="s">
         <v>25</v>
       </c>
-      <c r="G40" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G40" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" s="1">
         <v>8</v>
@@ -1726,13 +2011,16 @@
       <c r="F41" t="s">
         <v>10</v>
       </c>
-      <c r="G41" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G41" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" s="5">
         <v>9</v>
@@ -1749,13 +2037,16 @@
       <c r="F42" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G42" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="5">
         <v>9</v>
@@ -1772,13 +2063,16 @@
       <c r="F43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G43" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G43" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="5">
         <v>9</v>
@@ -1795,13 +2089,16 @@
       <c r="F44" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G44" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G44" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" s="5">
         <v>9</v>
@@ -1818,13 +2115,16 @@
       <c r="F45" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G45" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G45" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B46" s="5">
         <v>9</v>
@@ -1841,13 +2141,16 @@
       <c r="F46" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G46" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="B47" s="1">
         <v>10</v>
@@ -1864,13 +2167,16 @@
       <c r="F47" t="s">
         <v>14</v>
       </c>
-      <c r="G47" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G47" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B48" s="1">
         <v>10</v>
@@ -1887,13 +2193,16 @@
       <c r="F48" t="s">
         <v>12</v>
       </c>
-      <c r="G48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G48" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>164</v>
       </c>
       <c r="B49" s="1">
         <v>10</v>
@@ -1910,13 +2219,16 @@
       <c r="F49" t="s">
         <v>15</v>
       </c>
-      <c r="G49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G49" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>167</v>
       </c>
       <c r="B50" s="1">
         <v>10</v>
@@ -1933,13 +2245,16 @@
       <c r="F50" t="s">
         <v>10</v>
       </c>
-      <c r="G50" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G50" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="H50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B51" s="1">
         <v>10</v>
@@ -1956,12 +2271,67 @@
       <c r="F51" t="s">
         <v>11</v>
       </c>
-      <c r="G51" t="s">
-        <v>66</v>
+      <c r="G51" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="H51" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{CE42E53C-10B7-4E46-925F-BC5B0A968EFA}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{3F9EA1E3-282E-4DEA-B63C-A5BBEE7F61F4}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{4FA2F3CC-775C-405E-8D7C-3E7F5A75AAB8}"/>
+    <hyperlink ref="G7" r:id="rId4" xr:uid="{BE68D8D8-0331-428C-AEB6-D718BB1750A6}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{0DC4695C-72B5-44AA-80A6-6E7D99B89144}"/>
+    <hyperlink ref="G5" r:id="rId6" xr:uid="{70F520F1-31D4-4550-8C5A-BA4F13C1396E}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{8B5C306F-8399-4CFD-A5A4-332CCC75810F}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{451DFD88-FF8C-4109-97FD-64184F27DF21}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{246E7444-FA6F-46AC-84BA-8E6FE77ECEE1}"/>
+    <hyperlink ref="G11" r:id="rId10" xr:uid="{3E8E7576-F252-4EB5-BF2A-62F6A0EA210F}"/>
+    <hyperlink ref="G12" r:id="rId11" xr:uid="{E7366FB5-AF0C-4E76-8187-FA17175B1AB0}"/>
+    <hyperlink ref="G13" r:id="rId12" xr:uid="{BFE0CB4C-8938-4F6A-BC70-93BC36F919FC}"/>
+    <hyperlink ref="G14" r:id="rId13" xr:uid="{FB2BB3AC-002F-4D28-A2F1-215D90CAEB7C}"/>
+    <hyperlink ref="G15" r:id="rId14" xr:uid="{FE963BD1-96C4-459B-8B77-6C008D2127C6}"/>
+    <hyperlink ref="G16" r:id="rId15" xr:uid="{01EC07B7-B003-44F5-B197-C2049DDACBB5}"/>
+    <hyperlink ref="G17" r:id="rId16" xr:uid="{6F5FB8E3-9EDE-4DE7-BC1B-6BC84A40F266}"/>
+    <hyperlink ref="G18" r:id="rId17" xr:uid="{3E55BBA3-4A49-477C-8B7C-DCEC071FA6C5}"/>
+    <hyperlink ref="G19" r:id="rId18" xr:uid="{68B2BAD0-5A9F-4D8A-8915-FA25F4C3FB6C}"/>
+    <hyperlink ref="G20" r:id="rId19" xr:uid="{27C06BF5-0AD0-4C6C-9BAF-8AAE59A26A7D}"/>
+    <hyperlink ref="G21" r:id="rId20" xr:uid="{18335AC3-72DE-4815-A097-E492A178879D}"/>
+    <hyperlink ref="G22" r:id="rId21" xr:uid="{F4C6FDD8-8106-441C-BCF7-D38F2A14A3A7}"/>
+    <hyperlink ref="G23" r:id="rId22" xr:uid="{8D3E9E35-FE68-4D4A-AF57-A95773252A4C}"/>
+    <hyperlink ref="G24" r:id="rId23" xr:uid="{020C0587-2D94-4AAD-BA9D-9ABF96BC7FED}"/>
+    <hyperlink ref="G25" r:id="rId24" xr:uid="{796D3A55-0327-4D56-99F8-9E380A70A629}"/>
+    <hyperlink ref="G26" r:id="rId25" xr:uid="{E159039D-387F-45D2-B55C-5A8A68B83516}"/>
+    <hyperlink ref="G27" r:id="rId26" xr:uid="{D6EE8F79-4EB5-4B2C-84C2-159364FDDF2E}"/>
+    <hyperlink ref="G28" r:id="rId27" xr:uid="{251F031C-E7CE-47BE-AB43-8801C67D99C6}"/>
+    <hyperlink ref="G29" r:id="rId28" xr:uid="{324400C6-FB5E-4F77-A794-827B334A5F74}"/>
+    <hyperlink ref="G30" r:id="rId29" xr:uid="{67C41056-8276-4777-AA5F-28909A880CF7}"/>
+    <hyperlink ref="G31" r:id="rId30" xr:uid="{FAC6248D-1B9F-455B-97AC-94B72742EF6C}"/>
+    <hyperlink ref="G32" r:id="rId31" xr:uid="{59AEC4D2-86D1-47AC-B31F-FE282D5A8BDB}"/>
+    <hyperlink ref="G33" r:id="rId32" xr:uid="{2697B708-FEB6-4A85-A498-753F6F34A1F7}"/>
+    <hyperlink ref="G34" r:id="rId33" xr:uid="{C1F80A65-E64C-434F-8FEB-DB0AE3F52A06}"/>
+    <hyperlink ref="G35" r:id="rId34" xr:uid="{54E780C6-2AC8-49ED-B99F-C409BB657878}"/>
+    <hyperlink ref="G36" r:id="rId35" xr:uid="{70DF04F0-B84E-451E-9630-A6F5240AABE5}"/>
+    <hyperlink ref="G37" r:id="rId36" xr:uid="{CD6B7389-0071-410F-842E-32613DB4338D}"/>
+    <hyperlink ref="G38" r:id="rId37" xr:uid="{149A4C8E-D9D4-4AAD-ADB7-2B4EE249490C}"/>
+    <hyperlink ref="G39" r:id="rId38" xr:uid="{63F47EF6-0315-47E7-9DCB-323A244FDDE5}"/>
+    <hyperlink ref="G40" r:id="rId39" xr:uid="{FA8DFF6A-5A8E-4B8C-B035-03F3010B0950}"/>
+    <hyperlink ref="G41" r:id="rId40" xr:uid="{6C5786E6-51F1-4079-A0A5-940E4E133A4E}"/>
+    <hyperlink ref="G42" r:id="rId41" xr:uid="{9E02CF8B-8EC2-4FB6-8D47-570113270458}"/>
+    <hyperlink ref="G43" r:id="rId42" xr:uid="{4FA9262A-37A3-4EB2-9381-2BCF8B471B35}"/>
+    <hyperlink ref="G44" r:id="rId43" xr:uid="{333B4E02-D937-4AFB-A7E2-B7C3E863EEDA}"/>
+    <hyperlink ref="G45" r:id="rId44" xr:uid="{E1499CC8-A745-48F3-A8A1-65D509EFAC92}"/>
+    <hyperlink ref="G46" r:id="rId45" xr:uid="{3DF4D65D-0C1F-4E30-9611-F390F34E3447}"/>
+    <hyperlink ref="G47" r:id="rId46" xr:uid="{64D40201-FFEF-49D0-A8C5-69CE8CBB1E77}"/>
+    <hyperlink ref="G48" r:id="rId47" xr:uid="{D34CB1F8-258F-4CF9-AD08-ACEC5239CD9E}"/>
+    <hyperlink ref="G49" r:id="rId48" xr:uid="{9C8DA2D6-0125-4B44-A922-DC2E270922FE}"/>
+    <hyperlink ref="G50" r:id="rId49" xr:uid="{0D194E4D-80DF-4E1C-B355-BBCD5B35C651}"/>
+    <hyperlink ref="G51" r:id="rId50" xr:uid="{1F39884B-BEEF-4B1B-8127-37B816CD210D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>